<commit_message>
update program and presentation
</commit_message>
<xml_diff>
--- a/Data/Tags/colnames_M.xlsx
+++ b/Data/Tags/colnames_M.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcastillot/Library/CloudStorage/Dropbox/Tesis/2021/Italy/Urbino/Data/Repos/bibliometrix_dd_europe/Data/Tags_fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcastillot/Library/CloudStorage/Dropbox/Tesis/2021/Italy/Urbino/Data/Repos/Bibliometric_workshop/Data/Tags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEFCAF6-7FF5-7544-BF6C-2707FC87AE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565D916E-F780-9640-A2E2-0C841BE4CC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{8C18829D-5EEE-784D-B6AA-2299EA91AFE7}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="16300" xr2:uid="{8C18829D-5EEE-784D-B6AA-2299EA91AFE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Index</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Publication Name</t>
   </si>
   <si>
-    <t>JI</t>
-  </si>
-  <si>
-    <t>ISO Source Abbreviation</t>
-  </si>
-  <si>
     <t>DT</t>
   </si>
   <si>
@@ -119,18 +113,6 @@
     <t>Year Published</t>
   </si>
   <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>Research Areas</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>Accession Number</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -164,15 +146,6 @@
     <t>International Standard Book Number (ISBN)</t>
   </si>
   <si>
-    <t>WC</t>
-  </si>
-  <si>
-    <t>Web of Science Categories</t>
-  </si>
-  <si>
-    <t>Z9</t>
-  </si>
-  <si>
     <t>PU</t>
   </si>
   <si>
@@ -185,46 +158,43 @@
     <t>Funding Agency and Grant Number</t>
   </si>
   <si>
+    <t>Var name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Data Base</t>
+  </si>
+  <si>
+    <t>Authors affiliations</t>
+  </si>
+  <si>
+    <t>Corresponding Author affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author year journal </t>
+  </si>
+  <si>
+    <t>Author year journal full</t>
+  </si>
+  <si>
+    <t>Authors country</t>
+  </si>
+  <si>
+    <t>Var Type</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
     <t>PF</t>
   </si>
   <si>
-    <t>Platforms (WoS, Scopus Dimensions)</t>
-  </si>
-  <si>
-    <t>Var name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Times Cited Count </t>
-  </si>
-  <si>
-    <t>Data Base</t>
-  </si>
-  <si>
-    <t>Authors affiliations</t>
-  </si>
-  <si>
-    <t>Corresponding Author affiliation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author year journal </t>
-  </si>
-  <si>
-    <t>Author year journal full</t>
-  </si>
-  <si>
-    <t>Authors country</t>
-  </si>
-  <si>
-    <t>Var Type</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Numeric</t>
+    <t>Platform (Web of Science or Scopus)</t>
   </si>
 </sst>
 </file>
@@ -585,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2310A306-E68C-FB4F-9BE1-FE341F338901}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,13 +573,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -637,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -651,7 +621,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -659,13 +629,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -673,13 +643,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,13 +657,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -701,13 +671,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -715,13 +685,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -729,13 +699,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,13 +713,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -757,13 +727,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -771,13 +741,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,10 +758,10 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -799,13 +769,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,13 +783,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,13 +797,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,13 +808,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -855,13 +822,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,10 +836,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -880,13 +850,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -894,13 +864,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -908,13 +878,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
-        <v>59</v>
-      </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -928,7 +898,7 @@
         <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -936,83 +906,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>